<commit_message>
Final no mover nada de validaciones
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2E4Q4LA\Documents\UiPath\GeneracionCorreos_Beeckerco\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2E4Q4LA\Documents\UiPath\Generacion-Correo-Equipo-4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AA5B7B-F52C-4268-9824-2D7AA2BC0FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6A228C-0C51-49B5-8B7B-A7EF2F97FA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -192,15 +192,9 @@
     <t>ivan.garcia@beeckerco.com</t>
   </si>
   <si>
-    <t>eunice.hernandez@beeckerco.com</t>
-  </si>
-  <si>
     <t>EmailIvan</t>
   </si>
   <si>
-    <t>EmailEunice</t>
-  </si>
-  <si>
     <t>URL de donde se descarga la hoja de recursos para la obtencion de los nombres</t>
   </si>
   <si>
@@ -232,6 +226,30 @@
   </si>
   <si>
     <t>C:\Users\2E4Q4LA\Documents\UiPath\GeneracionCorreos_Beeckerco\Data</t>
+  </si>
+  <si>
+    <t>EmailS</t>
+  </si>
+  <si>
+    <t>{"eunice.hernandez@beeckerco.com","allisson.flores@beeckerco.com","angel.ramirez@beeckerco.com"}</t>
+  </si>
+  <si>
+    <t>Archivo procesado</t>
+  </si>
+  <si>
+    <t>Archivo  no procesado</t>
+  </si>
+  <si>
+    <t>C:\Users\2E4Q4LA\Documents\UiPath\GeneracionCorreos_Beeckerco\Data\Archivos_Generados\Procesados.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\2E4Q4LA\Documents\UiPath\GeneracionCorreos_Beeckerco\Data\Archivos_Generados\No procesados.xlsx</t>
+  </si>
+  <si>
+    <t>Ruta para tomar el archivo de procesados que se envia por correo</t>
+  </si>
+  <si>
+    <t>Ruta para tomar el archivo de  no procesados que se envia por correo</t>
   </si>
 </sst>
 </file>
@@ -357,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -399,15 +417,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -726,7 +743,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -823,36 +840,54 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:26" s="23" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A6" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="10"/>
     </row>
-    <row r="7" spans="1:26" ht="30">
-      <c r="A7" t="s">
+    <row r="9" spans="1:26" s="16" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" s="16" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="B10" s="14"/>
@@ -860,10 +895,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" s="7" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
@@ -873,41 +908,54 @@
         <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" s="8" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="22"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" t="s">
-        <v>59</v>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1">
+      <c r="B18" s="13"/>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1">
+      <c r="C19" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="17" customFormat="1" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B22" s="2"/>
+    </row>
     <row r="23" spans="1:3" s="15" customFormat="1" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1887,18 +1935,17 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="A20:XFD20"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A15:B15"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B16" r:id="rId1" xr:uid="{EDBBB762-857C-487B-AA03-AC9927E214A7}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{1332D643-9389-4085-9C36-BC7A1F28FB3D}"/>
+    <hyperlink ref="B17" r:id="rId2" display="eunice.hernandez@beeckerco.com" xr:uid="{1332D643-9389-4085-9C36-BC7A1F28FB3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -2118,24 +2165,24 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
         <v>64</v>
-      </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>